<commit_message>
added pics of built machine
</commit_message>
<xml_diff>
--- a/BOM/BillOfMaterials.xlsx
+++ b/BOM/BillOfMaterials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projs\onlygems\machine_cabbing\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F847B10A-A1B8-405F-93F4-3CA4988F1358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC5792A-6F57-40B4-82A8-31CA6502B4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{57779F7D-F035-47D5-90C4-63022A760CAE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{57779F7D-F035-47D5-90C4-63022A760CAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -988,7 +988,7 @@
   <dimension ref="A1:Y56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>